<commit_message>
Corrected overinflow computation to avoid pressurisation and axial flow
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09.xlsx
+++ b/simulations/inputs/Scenarios_24_09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242A491B-BF27-4FB4-8149-8C86550FA172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3276E8FB-AA17-4F3D-81F2-C44F3EA0EB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="578">
   <si>
     <t>input_file</t>
   </si>
@@ -1759,6 +1759,15 @@
   </si>
   <si>
     <t>Apoplasmic water conductivity</t>
+  </si>
+  <si>
+    <t>diffusion_xylem</t>
+  </si>
+  <si>
+    <t>g.s-1.m-3</t>
+  </si>
+  <si>
+    <t>Diffusion paramenter for exchanges between xylem apoplasm and cortex symplasm</t>
   </si>
 </sst>
 </file>
@@ -2951,11 +2960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T224"/>
+  <dimension ref="A1:T225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E234" sqref="E234"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I229" sqref="I229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16154,40 +16163,40 @@
         <v>-100000</v>
       </c>
       <c r="I211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="J211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="K211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="L211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="M211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="N211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="O211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="P211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="Q211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="R211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="S211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
       <c r="T211" s="98">
-        <v>-30000</v>
+        <v>-100000</v>
       </c>
     </row>
     <row r="212" spans="1:20" x14ac:dyDescent="0.25">
@@ -16764,281 +16773,315 @@
     </row>
     <row r="221" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E221" s="96" t="s">
+        <v>577</v>
+      </c>
+      <c r="F221" s="96" t="s">
+        <v>576</v>
+      </c>
+      <c r="G221" s="98"/>
+      <c r="H221" s="98"/>
+      <c r="I221" s="98"/>
+      <c r="J221" s="98"/>
+      <c r="K221" s="98"/>
+      <c r="L221" s="98"/>
+      <c r="M221" s="98"/>
+      <c r="N221" s="98"/>
+      <c r="O221" s="98"/>
+      <c r="P221" s="98"/>
+      <c r="Q221" s="98"/>
+      <c r="R221" s="98"/>
+      <c r="S221" s="98"/>
+      <c r="T221" s="98"/>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="B221" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="E221" s="96" t="s">
+      <c r="B222" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E222" s="96" t="s">
         <v>561</v>
       </c>
-      <c r="F221" s="96" t="s">
+      <c r="F222" s="96" t="s">
         <v>562</v>
       </c>
-      <c r="G221" s="98">
+      <c r="G222" s="98">
         <f>2*0.00001</f>
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="H221" s="98">
+      <c r="H222" s="98">
         <f>2*0.00001</f>
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="I221" s="98">
+      <c r="I222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="J221" s="98">
+      <c r="J222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="K221" s="98">
+      <c r="K222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="L221" s="98">
+      <c r="L222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="M221" s="98">
+      <c r="M222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="N221" s="98">
+      <c r="N222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="O221" s="98">
+      <c r="O222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="P221" s="98">
+      <c r="P222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="Q221" s="98">
+      <c r="Q222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="R221" s="98">
+      <c r="R222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="S221" s="98">
+      <c r="S222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="T221" s="98">
+      <c r="T222" s="98">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="B222" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D222" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="E222" s="96" t="s">
+      <c r="B223" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E223" s="96" t="s">
         <v>573</v>
       </c>
-      <c r="F222" s="96" t="s">
+      <c r="F223" s="96" t="s">
         <v>524</v>
       </c>
-      <c r="G222" s="98">
+      <c r="G223" s="98">
         <f>0.00000000000001 * 1000</f>
         <v>9.9999999999999994E-12</v>
       </c>
-      <c r="H222" s="98">
+      <c r="H223" s="98">
         <f>0.00000000000001 * 1000</f>
         <v>9.9999999999999994E-12</v>
       </c>
-      <c r="I222" s="98">
+      <c r="I223" s="98">
         <f>0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="J222" s="98">
-        <f t="shared" ref="J222:T222" si="16">0.00000000000001*10000*8</f>
+      <c r="J223" s="98">
+        <f t="shared" ref="J223:T223" si="16">0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="K222" s="98">
+      <c r="K223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="L222" s="98">
+      <c r="L223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="M222" s="98">
+      <c r="M223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="N222" s="98">
+      <c r="N223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="O222" s="98">
+      <c r="O223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="P222" s="98">
+      <c r="P223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="Q222" s="98">
+      <c r="Q223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="R222" s="98">
+      <c r="R223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="S222" s="98">
+      <c r="S223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
-      <c r="T222" s="98">
+      <c r="T223" s="98">
         <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
     </row>
-    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="B223" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D223" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="E223" s="96" t="s">
+      <c r="B224" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E224" s="96" t="s">
         <v>574</v>
       </c>
-      <c r="F223" s="96" t="s">
+      <c r="F224" s="96" t="s">
         <v>570</v>
       </c>
-      <c r="G223" s="98">
+      <c r="G224" s="98">
         <f>0.00000000000001 * 10000</f>
         <v>1E-10</v>
       </c>
-      <c r="H223" s="98">
+      <c r="H224" s="98">
         <f>0.00000000000001 * 10000</f>
         <v>1E-10</v>
       </c>
-      <c r="I223" s="98">
-        <f>I222*10</f>
+      <c r="I224" s="98">
+        <f>I223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="J223" s="98">
-        <f t="shared" ref="J223:T223" si="17">J222*10</f>
+      <c r="J224" s="98">
+        <f t="shared" ref="J224:T224" si="17">J223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="K223" s="98">
+      <c r="K224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="L223" s="98">
+      <c r="L224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="M223" s="98">
+      <c r="M224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="N223" s="98">
+      <c r="N224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="O223" s="98">
+      <c r="O224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="P223" s="98">
+      <c r="P224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="Q223" s="98">
+      <c r="Q224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="R223" s="98">
+      <c r="R224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="S223" s="98">
+      <c r="S224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="T223" s="98">
+      <c r="T224" s="98">
         <f t="shared" si="17"/>
         <v>8.0000000000000005E-9</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="B224" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D224" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="E224" s="96" t="s">
+      <c r="B225" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E225" s="96" t="s">
         <v>572</v>
       </c>
-      <c r="F224" s="96" t="s">
+      <c r="F225" s="96" t="s">
         <v>506</v>
       </c>
-      <c r="G224" s="98">
+      <c r="G225" s="98">
         <f>0.84*(0.36^2)</f>
         <v>0.10886399999999999</v>
       </c>
-      <c r="H224" s="98">
+      <c r="H225" s="98">
         <f>0.84*(0.36^2)</f>
         <v>0.10886399999999999</v>
       </c>
-      <c r="I224" s="98">
+      <c r="I225" s="98">
         <v>10</v>
       </c>
-      <c r="J224" s="98">
+      <c r="J225" s="98">
         <v>10</v>
       </c>
-      <c r="K224" s="98">
+      <c r="K225" s="98">
         <v>10</v>
       </c>
-      <c r="L224" s="98">
+      <c r="L225" s="98">
         <v>10</v>
       </c>
-      <c r="M224" s="98">
+      <c r="M225" s="98">
         <v>10</v>
       </c>
-      <c r="N224" s="98">
+      <c r="N225" s="98">
         <v>10</v>
       </c>
-      <c r="O224" s="98">
+      <c r="O225" s="98">
         <v>10</v>
       </c>
-      <c r="P224" s="98">
+      <c r="P225" s="98">
         <v>10</v>
       </c>
-      <c r="Q224" s="98">
+      <c r="Q225" s="98">
         <v>10</v>
       </c>
-      <c r="R224" s="98">
+      <c r="R225" s="98">
         <v>10</v>
       </c>
-      <c r="S224" s="98">
+      <c r="S225" s="98">
         <v>10</v>
       </c>
-      <c r="T224" s="98">
+      <c r="T225" s="98">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed useless volume extension
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09.xlsx
+++ b/simulations/inputs/Scenarios_24_09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3276E8FB-AA17-4F3D-81F2-C44F3EA0EB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB622D6-EF82-4397-B84C-FC313D0F96C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2963,8 +2963,8 @@
   <dimension ref="A1:T225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I229" sqref="I229"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F232" sqref="F232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16897,11 +16897,11 @@
         <v>9.9999999999999994E-12</v>
       </c>
       <c r="I223" s="98">
-        <f>0.00000000000001*10000*8</f>
+        <f t="shared" ref="I223:T223" si="16">0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="J223" s="98">
-        <f t="shared" ref="J223:T223" si="16">0.00000000000001*10000*8</f>
+        <f t="shared" si="16"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="K223" s="98">
@@ -16973,51 +16973,51 @@
         <v>1E-10</v>
       </c>
       <c r="I224" s="98">
-        <f>I223*10</f>
+        <f t="shared" ref="I224" si="17">I223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="J224" s="98">
-        <f t="shared" ref="J224:T224" si="17">J223*10</f>
+        <f t="shared" ref="J224:T224" si="18">J223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="K224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="L224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="M224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="N224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="O224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="P224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="Q224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="R224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="S224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="T224" s="98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.0000000000000005E-9</v>
       </c>
     </row>

</xml_diff>